<commit_message>
Add lab5 folder and fixing lab4
</commit_message>
<xml_diff>
--- a/Lab4_BVT/Lab4_663380223-3.xlsx
+++ b/Lab4_BVT/Lab4_663380223-3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GE\SoftwareQuality\lab\SQA\Assignment\Lab4_BVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\663380223-3\Lab5\cloneSelf\lab_cp353201\Lab4_BVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43753C8F-C678-4A66-90CD-292FA1F012C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="4" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="85">
   <si>
     <t>Test Case Design and Test Results</t>
   </si>
@@ -176,9 +177,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Gold</t>
-  </si>
-  <si>
     <t>TC01</t>
   </si>
   <si>
@@ -236,45 +234,12 @@
     <t>TC19</t>
   </si>
   <si>
-    <t>TC20</t>
-  </si>
-  <si>
     <t>Silver</t>
   </si>
   <si>
-    <t>Platinum</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
     <t>Invalid</t>
   </si>
   <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>TC26</t>
-  </si>
-  <si>
-    <t>TC27</t>
-  </si>
-  <si>
-    <t>TC28</t>
-  </si>
-  <si>
-    <t>Special Value Test case</t>
-  </si>
-  <si>
     <t>663380223-3</t>
   </si>
   <si>
@@ -282,12 +247,6 @@
   </si>
   <si>
     <t>15/07/2568</t>
-  </si>
-  <si>
-    <t>Special Silver Test case</t>
-  </si>
-  <si>
-    <t>Special Platinum Test case</t>
   </si>
   <si>
     <t>นายพิรัชย์ ชัยรัตน์ 663380223-3 Sec 1</t>
@@ -334,7 +293,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="12"/>
@@ -395,7 +354,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,18 +394,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +476,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,6 +524,33 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,46 +583,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 4" xfId="1"/>
-    <cellStyle name="Normal_ftest" xfId="2"/>
+    <cellStyle name="Normal 3 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_ftest" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -979,11 +920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="27.75"/>
@@ -1023,18 +964,18 @@
         <v>45</v>
       </c>
       <c r="B3" s="3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="41" t="s">
-        <v>98</v>
+      <c r="G3" s="23" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1042,18 +983,18 @@
         <v>46</v>
       </c>
       <c r="B4" s="3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1070,24 +1011,24 @@
         <v>43</v>
       </c>
       <c r="B6" s="3">
-        <v>45</v>
-      </c>
-      <c r="C6" s="38">
-        <v>9</v>
-      </c>
-      <c r="D6" s="39">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="C6" s="20">
+        <v>12</v>
+      </c>
+      <c r="D6" s="21">
+        <v>20</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="A9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1098,11 +1039,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
@@ -1120,15 +1061,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3" t="s">
         <v>23</v>
@@ -1159,82 +1100,82 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="3">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="L3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="3">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="L4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="3">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="L5" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="M5" s="3">
         <v>550</v>
@@ -1248,28 +1189,28 @@
         <v>99999</v>
       </c>
       <c r="L6" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="M6" s="3">
         <v>999</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24.95" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="38" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -1279,14 +1220,14 @@
         <v>100000</v>
       </c>
       <c r="L7" s="3">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="M7" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="28"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1296,9 +1237,9 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
       <c r="J8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1314,13 +1255,13 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
         <v>550</v>
@@ -1329,21 +1270,21 @@
         <v>48</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3">
         <v>550</v>
@@ -1352,30 +1293,30 @@
         <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C11" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3">
         <v>550</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>39</v>
@@ -1383,22 +1324,22 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3">
         <v>99999</v>
       </c>
       <c r="C12" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3">
         <v>550</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>39</v>
@@ -1406,13 +1347,13 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3">
         <v>100000</v>
       </c>
       <c r="C13" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3">
         <v>550</v>
@@ -1421,7 +1362,7 @@
         <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>39</v>
@@ -1432,13 +1373,13 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3">
         <v>550</v>
@@ -1458,13 +1399,13 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
         <v>550</v>
@@ -1473,10 +1414,10 @@
         <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1484,13 +1425,13 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C16" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3">
         <v>550</v>
@@ -1499,7 +1440,7 @@
         <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>39</v>
@@ -1510,13 +1451,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C17" s="3">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3">
         <v>550</v>
@@ -1525,7 +1466,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>39</v>
@@ -1536,86 +1477,82 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C18" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C19" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C20" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3">
         <v>999</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="1" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C21" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3">
         <v>1000</v>
@@ -1624,105 +1561,9 @@
         <v>48</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="34"/>
-      <c r="J21" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>100</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="3">
-        <v>49999</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>499</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C24" s="3">
-        <v>6</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C25" s="3">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1744,11 +1585,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
@@ -1766,15 +1607,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3" t="s">
         <v>23</v>
@@ -1792,95 +1633,95 @@
         <v>11</v>
       </c>
       <c r="K2" s="3">
-        <v>9999</v>
+        <v>-1</v>
       </c>
       <c r="L2" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M2" s="3">
-        <v>99</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="3">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="L3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="3">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="L4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="3">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="L5" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="M5" s="3">
         <v>550</v>
@@ -1894,28 +1735,28 @@
         <v>99999</v>
       </c>
       <c r="L6" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="M6" s="3">
         <v>999</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24.95" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="38" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -1925,14 +1766,14 @@
         <v>100000</v>
       </c>
       <c r="L7" s="3">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="M7" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="28"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1942,9 +1783,9 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
       <c r="J8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1952,7 +1793,7 @@
         <v>100001</v>
       </c>
       <c r="L8" s="3">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="M8" s="3">
         <v>1001</v>
@@ -1960,36 +1801,36 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3">
-        <v>9999</v>
+        <v>-1</v>
       </c>
       <c r="C9" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
         <v>550</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3">
         <v>550</v>
@@ -1998,21 +1839,21 @@
         <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3">
         <v>550</v>
@@ -2021,30 +1862,30 @@
         <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="37">
-        <v>55000</v>
-      </c>
-      <c r="C12" s="37">
-        <v>4</v>
-      </c>
-      <c r="D12" s="37">
+        <v>52</v>
+      </c>
+      <c r="B12" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C12" s="3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="19">
         <v>550</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>39</v>
@@ -2052,22 +1893,22 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3">
         <v>99999</v>
       </c>
       <c r="C13" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3">
         <v>550</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>39</v>
@@ -2075,13 +1916,13 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3">
         <v>100000</v>
       </c>
       <c r="C14" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3">
         <v>550</v>
@@ -2090,7 +1931,7 @@
         <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>39</v>
@@ -2098,13 +1939,13 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3">
         <v>100001</v>
       </c>
       <c r="C15" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3">
         <v>550</v>
@@ -2113,7 +1954,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>39</v>
@@ -2121,36 +1962,36 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D16" s="3">
         <v>550</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3">
         <v>550</v>
@@ -2165,15 +2006,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>550</v>
@@ -2182,21 +2023,21 @@
         <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C19" s="3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D19" s="3">
         <v>550</v>
@@ -2205,21 +2046,21 @@
         <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C20" s="3">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D20" s="3">
         <v>550</v>
@@ -2228,21 +2069,21 @@
         <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C21" s="3">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D21" s="3">
         <v>550</v>
@@ -2251,113 +2092,113 @@
         <v>48</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C22" s="3">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3">
-        <v>99</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="B23" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C23" s="3">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C23" s="3">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3">
-        <v>100</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C24" s="3">
+        <v>16</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C24" s="3">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3">
-        <v>101</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="B25" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C25" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D25" s="3">
         <v>999</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C26" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3">
         <v>1000</v>
@@ -2366,21 +2207,21 @@
         <v>48</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:7">
       <c r="A27" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="3">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="C27" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3">
         <v>1001</v>
@@ -2389,229 +2230,10 @@
         <v>48</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3">
-        <v>100</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="3">
-        <v>49999</v>
-      </c>
-      <c r="C29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29" s="3">
-        <v>499</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="32"/>
-      <c r="J29" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C30" s="3">
-        <v>6</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C31" s="3">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I31" s="35"/>
-      <c r="J31" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="3">
-        <v>-1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>4</v>
-      </c>
-      <c r="D32" s="3">
-        <v>550</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C33" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D33" s="3">
-        <v>550</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C34" s="3">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3">
-        <v>-1</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="3">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3">
-        <v>550</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="3">
-        <v>55000</v>
-      </c>
-      <c r="C36" s="3">
-        <v>4</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2631,11 +2253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
@@ -2692,71 +2314,71 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="40" t="s">
-        <v>93</v>
+      <c r="K3" s="22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="83.25">
-      <c r="A4" s="42">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="24">
         <v>2</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42" t="s">
-        <v>83</v>
+      <c r="C4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="40" t="s">
-        <v>94</v>
+      <c r="K4" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="111">
-      <c r="A5" s="42">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="24">
         <v>3</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42" t="s">
-        <v>83</v>
+      <c r="C5" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="40" t="s">
-        <v>96</v>
+      <c r="K5" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>